<commit_message>
Adding in process 2 files
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -133,8 +133,8 @@
     <col min="18" max="18" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="1.04296875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="1.04296875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="2.19921875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="2.19921875" customWidth="true" bestFit="true"/>
@@ -143,8 +143,8 @@
     <col min="28" max="28" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="2.19921875" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="2.19921875" customWidth="true" bestFit="true"/>
-    <col min="32" max="32" width="2.19921875" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="1.04296875" customWidth="true" bestFit="true"/>
+    <col min="32" max="32" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="33" max="33" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="34" max="34" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="1.04296875" customWidth="true" bestFit="true"/>
@@ -5291,19 +5291,19 @@
         <v>12</v>
       </c>
       <c r="U3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="V3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="W3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="X3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Y3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Z3" t="s">
         <v>12</v>
@@ -7489,22 +7489,22 @@
         <v>12</v>
       </c>
       <c r="W4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="X4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Y4" t="s">
         <v>13</v>
       </c>
       <c r="Z4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AA4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AB4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AC4" t="s">
         <v>12</v>
@@ -9690,10 +9690,10 @@
         <v>12</v>
       </c>
       <c r="Z5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AA5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AB5" t="s">
         <v>14</v>
@@ -9705,10 +9705,10 @@
         <v>14</v>
       </c>
       <c r="AE5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AF5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AG5" t="s">
         <v>12</v>
@@ -11894,13 +11894,13 @@
         <v>12</v>
       </c>
       <c r="AD6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AE6" t="s">
         <v>12</v>
       </c>
       <c r="AF6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AG6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Updating to handle date and file count validations
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18758" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18758" uniqueCount="27">
   <si>
     <t>JANUARY</t>
   </si>
@@ -65,28 +65,34 @@
     <t>5</t>
   </si>
   <si>
-    <t>8</t>
+    <t>10</t>
   </si>
   <si>
-    <t>10</t>
+    <t>7</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>13</t>
+    <t>8</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>7</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
   <si>
     <t>15</t>
-  </si>
-  <si>
-    <t>11</t>
   </si>
 </sst>
 </file>
@@ -182,7 +188,7 @@
     <col min="28" max="28" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="3.359375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="2.19921875" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="3.359375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="32" max="32" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="33" max="33" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="34" max="34" width="2.19921875" customWidth="true" bestFit="true"/>
@@ -190,7 +196,7 @@
     <col min="36" max="36" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="3.359375" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="3.359375" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="3.359375" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="41" max="41" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="42" max="42" width="2.19921875" customWidth="true" bestFit="true"/>
@@ -202,7 +208,7 @@
     <col min="48" max="48" width="3.359375" customWidth="true" bestFit="true"/>
     <col min="49" max="49" width="3.359375" customWidth="true" bestFit="true"/>
     <col min="50" max="50" width="3.359375" customWidth="true" bestFit="true"/>
-    <col min="51" max="51" width="3.359375" customWidth="true" bestFit="true"/>
+    <col min="51" max="51" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="52" max="52" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="53" max="53" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="54" max="54" width="2.19921875" customWidth="true" bestFit="true"/>
@@ -222,8 +228,8 @@
     <col min="68" max="68" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="69" max="69" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="70" max="70" width="2.19921875" customWidth="true" bestFit="true"/>
-    <col min="71" max="71" width="2.19921875" customWidth="true" bestFit="true"/>
-    <col min="72" max="72" width="2.19921875" customWidth="true" bestFit="true"/>
+    <col min="71" max="71" width="1.04296875" customWidth="true" bestFit="true"/>
+    <col min="72" max="72" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="73" max="73" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="74" max="74" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="75" max="75" width="1.04296875" customWidth="true" bestFit="true"/>
@@ -5329,14 +5335,14 @@
       <c r="T3" t="s">
         <v>12</v>
       </c>
-      <c r="U3" t="s">
-        <v>12</v>
-      </c>
-      <c r="V3" t="s">
-        <v>12</v>
+      <c r="U3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.0</v>
       </c>
       <c r="W3" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="X3" t="n">
         <v>0.0</v>
@@ -5348,7 +5354,7 @@
         <v>0.0</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="AB3" t="n">
         <v>0.0</v>
@@ -5356,11 +5362,11 @@
       <c r="AC3" t="n">
         <v>3.0</v>
       </c>
-      <c r="AD3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>3.0</v>
+      <c r="AD3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>12</v>
       </c>
       <c r="AF3" t="s">
         <v>12</v>
@@ -7545,11 +7551,11 @@
       <c r="AB4" t="s">
         <v>12</v>
       </c>
-      <c r="AC4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>12</v>
+      <c r="AC4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.0</v>
       </c>
       <c r="AE4" t="n">
         <v>0.0</v>
@@ -7564,19 +7570,19 @@
         <v>0.0</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="AJ4" t="n">
         <v>0.0</v>
       </c>
       <c r="AK4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AM4" t="n">
         <v>3.0</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>12</v>
       </c>
       <c r="AN4" t="s">
         <v>12</v>
@@ -9761,11 +9767,11 @@
       <c r="AJ5" t="s">
         <v>12</v>
       </c>
-      <c r="AK5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>12</v>
+      <c r="AK5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0.0</v>
       </c>
       <c r="AM5" t="n">
         <v>0.0</v>
@@ -9774,19 +9780,19 @@
         <v>0.0</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="AP5" t="n">
         <v>0.0</v>
       </c>
       <c r="AQ5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AS5" t="n">
         <v>3.0</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>12</v>
       </c>
       <c r="AT5" t="s">
         <v>12</v>
@@ -11971,11 +11977,11 @@
       <c r="AP6" t="s">
         <v>12</v>
       </c>
-      <c r="AQ6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>12</v>
+      <c r="AQ6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>0.0</v>
       </c>
       <c r="AS6" t="n">
         <v>0.0</v>
@@ -11984,19 +11990,19 @@
         <v>0.0</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="AV6" t="n">
         <v>0.0</v>
       </c>
       <c r="AW6" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="AX6" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AY6" t="n">
         <v>3.0</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>12</v>
       </c>
       <c r="AZ6" t="s">
         <v>12</v>
@@ -14181,11 +14187,11 @@
       <c r="AV7" t="s">
         <v>12</v>
       </c>
-      <c r="AW7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AX7" t="s">
-        <v>12</v>
+      <c r="AW7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>0.0</v>
       </c>
       <c r="AY7" t="n">
         <v>2.0</v>
@@ -14209,13 +14215,13 @@
         <v>2.0</v>
       </c>
       <c r="BF7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="BG7" t="n">
         <v>0.0</v>
       </c>
-      <c r="BG7" t="n">
-        <v>2.0</v>
-      </c>
       <c r="BH7" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="BI7" t="n">
         <v>0.0</v>
@@ -14224,16 +14230,16 @@
         <v>0.0</v>
       </c>
       <c r="BK7" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="BL7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="BM7" t="n">
         <v>4.0</v>
       </c>
-      <c r="BN7" t="n">
-        <v>4.0</v>
+      <c r="BM7" t="s">
+        <v>12</v>
+      </c>
+      <c r="BN7" t="s">
+        <v>12</v>
       </c>
       <c r="BO7" t="s">
         <v>12</v>
@@ -16391,23 +16397,23 @@
       <c r="BB8" t="s">
         <v>12</v>
       </c>
-      <c r="BC8" t="s">
-        <v>12</v>
-      </c>
-      <c r="BD8" t="s">
-        <v>12</v>
+      <c r="BC8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>5.0</v>
       </c>
       <c r="BE8" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="BF8" t="n">
         <v>5.0</v>
       </c>
       <c r="BG8" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="BH8" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="BI8" t="n">
         <v>2.0</v>
@@ -16416,10 +16422,10 @@
         <v>0.0</v>
       </c>
       <c r="BK8" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="BL8" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="BM8" t="n">
         <v>4.0</v>
@@ -16428,16 +16434,16 @@
         <v>4.0</v>
       </c>
       <c r="BO8" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="BP8" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="BQ8" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="BR8" t="n">
         <v>1.0</v>
+      </c>
+      <c r="BQ8" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR8" t="s">
+        <v>12</v>
       </c>
       <c r="BS8" t="s">
         <v>12</v>
@@ -18619,17 +18625,17 @@
       <c r="BN9" t="s">
         <v>12</v>
       </c>
-      <c r="BO9" t="s">
-        <v>12</v>
-      </c>
-      <c r="BP9" t="s">
-        <v>12</v>
-      </c>
-      <c r="BQ9" t="n">
+      <c r="BO9" t="n">
         <v>2.0</v>
       </c>
-      <c r="BR9" t="n">
+      <c r="BP9" t="n">
         <v>2.0</v>
+      </c>
+      <c r="BQ9" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR9" t="s">
+        <v>12</v>
       </c>
       <c r="BS9" t="s">
         <v>12</v>
@@ -20811,20 +20817,20 @@
       <c r="BN10" t="s">
         <v>12</v>
       </c>
-      <c r="BO10" t="s">
-        <v>12</v>
-      </c>
-      <c r="BP10" t="s">
-        <v>12</v>
+      <c r="BO10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="BP10" t="n">
+        <v>1.0</v>
       </c>
       <c r="BQ10" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="BR10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="BS10" t="n">
         <v>0.0</v>
+      </c>
+      <c r="BR10" t="s">
+        <v>12</v>
+      </c>
+      <c r="BS10" t="s">
+        <v>12</v>
       </c>
       <c r="BT10" t="s">
         <v>12</v>
@@ -23006,20 +23012,20 @@
       <c r="BO11" t="s">
         <v>12</v>
       </c>
-      <c r="BP11" t="s">
-        <v>12</v>
-      </c>
-      <c r="BQ11" t="s">
-        <v>12</v>
+      <c r="BP11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="BQ11" t="n">
+        <v>3.0</v>
       </c>
       <c r="BR11" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="BS11" t="n">
         <v>3.0</v>
       </c>
-      <c r="BT11" t="n">
-        <v>3.0</v>
+      <c r="BS11" t="s">
+        <v>12</v>
+      </c>
+      <c r="BT11" t="s">
+        <v>12</v>
       </c>
       <c r="BU11" t="s">
         <v>12</v>
@@ -25198,20 +25204,20 @@
       <c r="BO12" t="s">
         <v>12</v>
       </c>
-      <c r="BP12" t="s">
-        <v>12</v>
-      </c>
-      <c r="BQ12" t="s">
-        <v>12</v>
+      <c r="BP12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="BQ12" t="n">
+        <v>3.0</v>
       </c>
       <c r="BR12" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="BS12" t="n">
         <v>3.0</v>
       </c>
-      <c r="BT12" t="n">
-        <v>3.0</v>
+      <c r="BS12" t="s">
+        <v>12</v>
+      </c>
+      <c r="BT12" t="s">
+        <v>12</v>
       </c>
       <c r="BU12" t="s">
         <v>12</v>
@@ -27396,14 +27402,14 @@
       <c r="BQ13" t="s">
         <v>12</v>
       </c>
-      <c r="BR13" t="s">
-        <v>12</v>
+      <c r="BR13" t="n">
+        <v>1.0</v>
       </c>
       <c r="BS13" t="s">
         <v>12</v>
       </c>
-      <c r="BT13" t="n">
-        <v>1.0</v>
+      <c r="BT13" t="s">
+        <v>12</v>
       </c>
       <c r="BU13" t="s">
         <v>12</v>
@@ -57938,13 +57944,13 @@
         <v>12</v>
       </c>
       <c r="U27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="V27" t="s">
         <v>12</v>
       </c>
       <c r="W27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X27" t="s">
         <v>12</v>
@@ -57956,13 +57962,13 @@
         <v>12</v>
       </c>
       <c r="AA27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AB27" t="s">
         <v>12</v>
       </c>
       <c r="AC27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AD27" t="s">
         <v>12</v>
@@ -57980,58 +57986,58 @@
         <v>12</v>
       </c>
       <c r="AI27" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="AJ27" t="s">
         <v>16</v>
       </c>
       <c r="AK27" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>23</v>
+      </c>
+      <c r="AN27" t="s">
+        <v>18</v>
+      </c>
+      <c r="AO27" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR27" t="s">
         <v>20</v>
       </c>
-      <c r="AL27" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM27" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN27" t="s">
+      <c r="AS27" t="s">
         <v>22</v>
       </c>
-      <c r="AO27" t="s">
-        <v>19</v>
-      </c>
-      <c r="AP27" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ27" t="s">
-        <v>21</v>
-      </c>
-      <c r="AR27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AS27" t="s">
-        <v>23</v>
-      </c>
       <c r="AT27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AU27" t="s">
         <v>24</v>
       </c>
       <c r="AV27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AW27" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AX27" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="AY27" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="AZ27" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="BA27" t="s">
         <v>15</v>
@@ -58040,22 +58046,22 @@
         <v>12</v>
       </c>
       <c r="BC27" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD27" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE27" t="s">
+        <v>18</v>
+      </c>
+      <c r="BF27" t="s">
+        <v>18</v>
+      </c>
+      <c r="BG27" t="s">
         <v>15</v>
       </c>
-      <c r="BD27" t="s">
-        <v>12</v>
-      </c>
-      <c r="BE27" t="s">
-        <v>19</v>
-      </c>
-      <c r="BF27" t="s">
-        <v>16</v>
-      </c>
-      <c r="BG27" t="s">
-        <v>22</v>
-      </c>
       <c r="BH27" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="BI27" t="s">
         <v>15</v>
@@ -58064,34 +58070,34 @@
         <v>12</v>
       </c>
       <c r="BK27" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="BL27" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="BM27" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="BN27" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="BO27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="BP27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="BQ27" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="BR27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BS27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="BT27" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="BU27" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Update for Cell formating and date stagger
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -65,13 +65,19 @@
     <t>5</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
-    <t>4</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
   <si>
     <t>8</t>
@@ -80,19 +86,13 @@
     <t>14</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>18</t>
+    <t>16</t>
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -109,12 +109,72 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="46"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="46"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="24"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
@@ -124,6 +184,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="29"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="44"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
       </patternFill>
     </fill>
     <fill>
@@ -158,1484 +228,1484 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1676,7 +1746,7 @@
     <col min="26" max="26" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="2.19921875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="3.359375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="32" max="32" width="2.19921875" customWidth="true" bestFit="true"/>
@@ -1686,7 +1756,7 @@
     <col min="36" max="36" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="3.359375" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="3.359375" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="2.19921875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="3.359375" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="41" max="41" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="42" max="42" width="2.19921875" customWidth="true" bestFit="true"/>
@@ -1716,8 +1786,8 @@
     <col min="66" max="66" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="67" max="67" width="2.19921875" customWidth="true" bestFit="true"/>
     <col min="68" max="68" width="2.19921875" customWidth="true" bestFit="true"/>
-    <col min="69" max="69" width="2.19921875" customWidth="true" bestFit="true"/>
-    <col min="70" max="70" width="2.19921875" customWidth="true" bestFit="true"/>
+    <col min="69" max="69" width="1.04296875" customWidth="true" bestFit="true"/>
+    <col min="70" max="70" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="71" max="71" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="72" max="72" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="73" max="73" width="1.04296875" customWidth="true" bestFit="true"/>
@@ -6819,14 +6889,14 @@
       <c r="R3" t="s">
         <v>12</v>
       </c>
-      <c r="S3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T3" t="s">
-        <v>12</v>
+      <c r="S3" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="T3" t="n" s="2">
+        <v>0.0</v>
       </c>
       <c r="U3" t="n" s="2">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="V3" t="n" s="2">
         <v>0.0</v>
@@ -6838,7 +6908,7 @@
         <v>0.0</v>
       </c>
       <c r="Y3" t="n" s="2">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="Z3" t="n" s="2">
         <v>0.0</v>
@@ -6846,11 +6916,11 @@
       <c r="AA3" t="n" s="2">
         <v>3.0</v>
       </c>
-      <c r="AB3" t="n" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="AC3" t="n" s="2">
-        <v>3.0</v>
+      <c r="AB3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>12</v>
       </c>
       <c r="AD3" t="s">
         <v>12</v>
@@ -9035,11 +9105,11 @@
       <c r="Z4" t="s">
         <v>12</v>
       </c>
-      <c r="AA4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>12</v>
+      <c r="AA4" t="n" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="AB4" t="n" s="3">
+        <v>0.0</v>
       </c>
       <c r="AC4" t="n" s="3">
         <v>0.0</v>
@@ -9054,19 +9124,19 @@
         <v>0.0</v>
       </c>
       <c r="AG4" t="n" s="3">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="AH4" t="n" s="3">
         <v>0.0</v>
       </c>
       <c r="AI4" t="n" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="AJ4" t="n" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="AK4" t="n" s="3">
         <v>3.0</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>12</v>
       </c>
       <c r="AL4" t="s">
         <v>12</v>
@@ -11251,11 +11321,11 @@
       <c r="AH5" t="s">
         <v>12</v>
       </c>
-      <c r="AI5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>12</v>
+      <c r="AI5" t="n" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="AJ5" t="n" s="4">
+        <v>0.0</v>
       </c>
       <c r="AK5" t="n" s="4">
         <v>0.0</v>
@@ -11264,19 +11334,19 @@
         <v>0.0</v>
       </c>
       <c r="AM5" t="n" s="4">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="AN5" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="AO5" t="n" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="AP5" t="n" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="AQ5" t="n" s="4">
         <v>3.0</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>12</v>
       </c>
       <c r="AR5" t="s">
         <v>12</v>
@@ -13461,11 +13531,11 @@
       <c r="AN6" t="s">
         <v>12</v>
       </c>
-      <c r="AO6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>12</v>
+      <c r="AO6" t="n" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="AP6" t="n" s="5">
+        <v>0.0</v>
       </c>
       <c r="AQ6" t="n" s="5">
         <v>0.0</v>
@@ -13474,19 +13544,19 @@
         <v>0.0</v>
       </c>
       <c r="AS6" t="n" s="5">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="AT6" t="n" s="5">
         <v>0.0</v>
       </c>
       <c r="AU6" t="n" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="AV6" t="n" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="AW6" t="n" s="5">
         <v>3.0</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>12</v>
       </c>
       <c r="AX6" t="s">
         <v>12</v>
@@ -15671,11 +15741,11 @@
       <c r="AT7" t="n" s="6">
         <v>4.0</v>
       </c>
-      <c r="AU7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV7" t="s">
-        <v>12</v>
+      <c r="AU7" t="n" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="AV7" t="n" s="6">
+        <v>0.0</v>
       </c>
       <c r="AW7" t="n" s="6">
         <v>2.0</v>
@@ -15699,13 +15769,13 @@
         <v>2.0</v>
       </c>
       <c r="BD7" t="n" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="BE7" t="n" s="6">
         <v>0.0</v>
       </c>
-      <c r="BE7" t="n" s="6">
-        <v>2.0</v>
-      </c>
       <c r="BF7" t="n" s="6">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="BG7" t="n" s="6">
         <v>0.0</v>
@@ -15714,16 +15784,16 @@
         <v>0.0</v>
       </c>
       <c r="BI7" t="n" s="6">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="BJ7" t="n" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="BK7" t="n" s="6">
         <v>4.0</v>
       </c>
-      <c r="BL7" t="n" s="6">
-        <v>4.0</v>
+      <c r="BK7" t="s">
+        <v>12</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>12</v>
       </c>
       <c r="BM7" t="s">
         <v>12</v>
@@ -17881,23 +17951,23 @@
       <c r="AZ8" t="s">
         <v>12</v>
       </c>
-      <c r="BA8" t="s">
-        <v>12</v>
-      </c>
-      <c r="BB8" t="s">
-        <v>12</v>
+      <c r="BA8" t="n" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="BB8" t="n" s="7">
+        <v>5.0</v>
       </c>
       <c r="BC8" t="n" s="7">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="BD8" t="n" s="7">
         <v>5.0</v>
       </c>
       <c r="BE8" t="n" s="7">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="BF8" t="n" s="7">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="BG8" t="n" s="7">
         <v>2.0</v>
@@ -17906,10 +17976,10 @@
         <v>0.0</v>
       </c>
       <c r="BI8" t="n" s="7">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="BJ8" t="n" s="7">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="BK8" t="n" s="7">
         <v>4.0</v>
@@ -17918,16 +17988,16 @@
         <v>4.0</v>
       </c>
       <c r="BM8" t="n" s="7">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="BN8" t="n" s="7">
-        <v>4.0</v>
-      </c>
-      <c r="BO8" t="n" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="BP8" t="n" s="7">
         <v>1.0</v>
+      </c>
+      <c r="BO8" t="s">
+        <v>12</v>
+      </c>
+      <c r="BP8" t="s">
+        <v>12</v>
       </c>
       <c r="BQ8" t="s">
         <v>12</v>
@@ -20109,17 +20179,17 @@
       <c r="BL9" t="s">
         <v>12</v>
       </c>
-      <c r="BM9" t="s">
-        <v>12</v>
-      </c>
-      <c r="BN9" t="s">
-        <v>12</v>
-      </c>
-      <c r="BO9" t="n" s="8">
+      <c r="BM9" t="n" s="8">
         <v>2.0</v>
       </c>
-      <c r="BP9" t="n" s="8">
+      <c r="BN9" t="n" s="8">
         <v>2.0</v>
+      </c>
+      <c r="BO9" t="s">
+        <v>12</v>
+      </c>
+      <c r="BP9" t="s">
+        <v>12</v>
       </c>
       <c r="BQ9" t="s">
         <v>12</v>
@@ -22301,20 +22371,20 @@
       <c r="BL10" t="s">
         <v>12</v>
       </c>
-      <c r="BM10" t="s">
-        <v>12</v>
-      </c>
-      <c r="BN10" t="s">
-        <v>12</v>
+      <c r="BM10" t="n" s="9">
+        <v>2.0</v>
+      </c>
+      <c r="BN10" t="n" s="9">
+        <v>1.0</v>
       </c>
       <c r="BO10" t="n" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="BP10" t="n" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="BQ10" t="n" s="9">
         <v>0.0</v>
+      </c>
+      <c r="BP10" t="s">
+        <v>12</v>
+      </c>
+      <c r="BQ10" t="s">
+        <v>12</v>
       </c>
       <c r="BR10" t="s">
         <v>12</v>
@@ -24496,20 +24566,20 @@
       <c r="BM11" t="s">
         <v>12</v>
       </c>
-      <c r="BN11" t="s">
-        <v>12</v>
-      </c>
-      <c r="BO11" t="s">
-        <v>12</v>
+      <c r="BN11" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="BO11" t="n" s="10">
+        <v>3.0</v>
       </c>
       <c r="BP11" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="BQ11" t="n" s="10">
         <v>3.0</v>
       </c>
-      <c r="BR11" t="n" s="10">
-        <v>3.0</v>
+      <c r="BQ11" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR11" t="s">
+        <v>12</v>
       </c>
       <c r="BS11" t="s">
         <v>12</v>
@@ -26688,20 +26758,20 @@
       <c r="BM12" t="s">
         <v>12</v>
       </c>
-      <c r="BN12" t="s">
-        <v>12</v>
-      </c>
-      <c r="BO12" t="s">
-        <v>12</v>
+      <c r="BN12" t="n" s="11">
+        <v>2.0</v>
+      </c>
+      <c r="BO12" t="n" s="11">
+        <v>3.0</v>
       </c>
       <c r="BP12" t="n" s="11">
-        <v>2.0</v>
-      </c>
-      <c r="BQ12" t="n" s="11">
         <v>3.0</v>
       </c>
-      <c r="BR12" t="n" s="11">
-        <v>3.0</v>
+      <c r="BQ12" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR12" t="s">
+        <v>12</v>
       </c>
       <c r="BS12" t="s">
         <v>12</v>
@@ -28886,14 +28956,14 @@
       <c r="BO13" t="s">
         <v>12</v>
       </c>
-      <c r="BP13" t="s">
-        <v>12</v>
+      <c r="BP13" t="n" s="12">
+        <v>1.0</v>
       </c>
       <c r="BQ13" t="s">
         <v>12</v>
       </c>
-      <c r="BR13" t="n" s="12">
-        <v>1.0</v>
+      <c r="BR13" t="s">
+        <v>12</v>
       </c>
       <c r="BS13" t="s">
         <v>12</v>
@@ -59428,13 +59498,13 @@
         <v>12</v>
       </c>
       <c r="S27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T27" t="s">
         <v>12</v>
       </c>
       <c r="U27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="V27" t="s">
         <v>12</v>
@@ -59446,7 +59516,7 @@
         <v>12</v>
       </c>
       <c r="Y27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Z27" t="s">
         <v>12</v>
@@ -59464,88 +59534,88 @@
         <v>12</v>
       </c>
       <c r="AE27" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI27" t="s">
         <v>18</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG27" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI27" t="s">
-        <v>20</v>
       </c>
       <c r="AJ27" t="s">
         <v>16</v>
       </c>
       <c r="AK27" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN27" t="s">
+        <v>17</v>
+      </c>
+      <c r="AO27" t="s">
+        <v>17</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ27" t="s">
         <v>21</v>
       </c>
-      <c r="AL27" t="s">
+      <c r="AR27" t="s">
         <v>22</v>
       </c>
-      <c r="AM27" t="s">
+      <c r="AS27" t="s">
         <v>23</v>
       </c>
-      <c r="AN27" t="s">
-        <v>18</v>
-      </c>
-      <c r="AO27" t="s">
-        <v>14</v>
-      </c>
-      <c r="AP27" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ27" t="s">
-        <v>24</v>
-      </c>
-      <c r="AR27" t="s">
+      <c r="AT27" t="s">
         <v>20</v>
-      </c>
-      <c r="AS27" t="s">
-        <v>22</v>
-      </c>
-      <c r="AT27" t="s">
-        <v>22</v>
       </c>
       <c r="AU27" t="s">
         <v>24</v>
       </c>
       <c r="AV27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AW27" t="s">
         <v>25</v>
       </c>
       <c r="AX27" t="s">
+        <v>25</v>
+      </c>
+      <c r="AY27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ27" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA27" t="s">
         <v>26</v>
       </c>
-      <c r="AY27" t="s">
-        <v>20</v>
-      </c>
-      <c r="AZ27" t="s">
-        <v>18</v>
-      </c>
-      <c r="BA27" t="s">
+      <c r="BB27" t="s">
+        <v>16</v>
+      </c>
+      <c r="BC27" t="s">
+        <v>17</v>
+      </c>
+      <c r="BD27" t="s">
+        <v>17</v>
+      </c>
+      <c r="BE27" t="s">
         <v>15</v>
       </c>
-      <c r="BB27" t="s">
-        <v>12</v>
-      </c>
-      <c r="BC27" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD27" t="s">
-        <v>16</v>
-      </c>
-      <c r="BE27" t="s">
-        <v>18</v>
-      </c>
       <c r="BF27" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="BG27" t="s">
         <v>15</v>
@@ -59554,34 +59624,34 @@
         <v>12</v>
       </c>
       <c r="BI27" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="BJ27" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="BK27" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="BL27" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="BM27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="BN27" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="BO27" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="BP27" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="BQ27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="BR27" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="BS27" t="s">
         <v>12</v>

</xml_diff>